<commit_message>
add summary of tracer studies
</commit_message>
<xml_diff>
--- a/growth_chamber_progs/TT25_gc_program_all.xlsx
+++ b/growth_chamber_progs/TT25_gc_program_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/2025_TT_psf/growth_chamber_progs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5633E690-C769-DF49-B48D-CFC6091DC76B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BCAE6B-2AB4-534D-BCEA-529048C8D7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10000" yWindow="500" windowWidth="32840" windowHeight="26300" xr2:uid="{62858E1A-CBBA-F648-9C96-600253477C31}"/>
   </bookViews>
@@ -244,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -253,8 +253,9 @@
     <xf numFmtId="20" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -262,11 +263,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{485BC472-66D5-8C42-8BB7-D5B104E0FFF3}">
   <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -636,13 +635,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="10">
         <v>45644</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="10">
         <v>45669</v>
       </c>
       <c r="D2" s="5">
@@ -659,9 +658,9 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="2">
         <v>0.45833333333333331</v>
       </c>
@@ -676,9 +675,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="5">
         <v>0.79166666666666663</v>
       </c>
@@ -693,9 +692,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="2">
         <v>0.83333333333333337</v>
       </c>
@@ -710,9 +709,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="5">
         <v>0</v>
       </c>
@@ -750,13 +749,13 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="10">
         <v>45669</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="10">
         <v>45691</v>
       </c>
       <c r="D9" s="5">
@@ -773,9 +772,9 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
       <c r="D10" s="2">
         <v>0.4375</v>
       </c>
@@ -790,9 +789,9 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
       <c r="D11" s="5">
         <v>0.45833333333333331</v>
       </c>
@@ -807,9 +806,9 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
       <c r="D12" s="2">
         <v>0.875</v>
       </c>
@@ -824,9 +823,9 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
       <c r="D13" s="5">
         <v>0.89583333333333337</v>
       </c>
@@ -841,9 +840,9 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
       <c r="D14" s="2">
         <v>0.91666666666666663</v>
       </c>
@@ -858,9 +857,9 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
       <c r="D15" s="5">
         <v>0</v>
       </c>
@@ -898,14 +897,14 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="10">
         <v>45691</v>
       </c>
-      <c r="C18" s="9">
-        <v>45705</v>
+      <c r="C18" s="10">
+        <v>45698</v>
       </c>
       <c r="D18" s="5">
         <v>0.41666666666666669</v>
@@ -921,9 +920,9 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="8"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
       <c r="D19" s="2">
         <v>0.4375</v>
       </c>
@@ -938,9 +937,9 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="8"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
       <c r="D20" s="5">
         <v>0.45833333333333331</v>
       </c>
@@ -955,9 +954,9 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="8"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
       <c r="D21" s="2">
         <v>0.91666666666666663</v>
       </c>
@@ -972,9 +971,9 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="8"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
       <c r="D22" s="5">
         <v>0.9375</v>
       </c>
@@ -989,9 +988,9 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="8"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
       <c r="D23" s="2">
         <v>0.95833333333333337</v>
       </c>
@@ -1006,9 +1005,9 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="8"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
       <c r="D24" s="5">
         <v>0</v>
       </c>
@@ -1046,13 +1045,13 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="9">
-        <v>45705</v>
-      </c>
-      <c r="C27" s="9">
+      <c r="B27" s="10">
+        <v>45698</v>
+      </c>
+      <c r="C27" s="10">
         <v>45719</v>
       </c>
       <c r="D27" s="5">
@@ -1069,9 +1068,9 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="8"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
       <c r="D28" s="2">
         <v>0.4375</v>
       </c>
@@ -1086,9 +1085,9 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="8"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
       <c r="D29" s="5">
         <v>0.45833333333333331</v>
       </c>
@@ -1103,9 +1102,9 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="8"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
       <c r="D30" s="2">
         <v>0.91666666666666663</v>
       </c>
@@ -1120,9 +1119,9 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="8"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
       <c r="D31" s="5">
         <v>0.9375</v>
       </c>
@@ -1137,9 +1136,9 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="8"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
       <c r="D32" s="2">
         <v>0.95833333333333337</v>
       </c>
@@ -1154,9 +1153,9 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="8"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
       <c r="D33" s="5">
         <v>0</v>
       </c>
@@ -1194,13 +1193,13 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B36" s="9">
+      <c r="B36" s="10">
         <v>45719</v>
       </c>
-      <c r="C36" s="9">
+      <c r="C36" s="10">
         <v>45733</v>
       </c>
       <c r="D36" s="5">
@@ -1217,9 +1216,9 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="8"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
       <c r="D37" s="2">
         <v>0.4375</v>
       </c>
@@ -1234,9 +1233,9 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="8"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
       <c r="D38" s="5">
         <v>0.45833333333333331</v>
       </c>
@@ -1251,9 +1250,9 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="8"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
       <c r="D39" s="2">
         <v>0.91666666666666663</v>
       </c>
@@ -1268,9 +1267,9 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="8"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
       <c r="D40" s="5">
         <v>0.9375</v>
       </c>
@@ -1285,9 +1284,9 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="8"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
       <c r="D41" s="2">
         <v>0.95833333333333337</v>
       </c>
@@ -1302,9 +1301,9 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="8"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
       <c r="D42" s="5">
         <v>0</v>
       </c>
@@ -1342,13 +1341,13 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B45" s="9">
+      <c r="B45" s="10">
         <v>45733</v>
       </c>
-      <c r="C45" s="9">
+      <c r="C45" s="10">
         <v>45747</v>
       </c>
       <c r="D45" s="5">
@@ -1365,9 +1364,9 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="8"/>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10"/>
+      <c r="A46" s="12"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
       <c r="D46" s="2">
         <v>0.4375</v>
       </c>
@@ -1382,9 +1381,9 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="8"/>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
+      <c r="A47" s="12"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
       <c r="D47" s="5">
         <v>0.45833333333333331</v>
       </c>
@@ -1399,9 +1398,9 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="8"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
+      <c r="A48" s="12"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
       <c r="D48" s="2">
         <v>0.91666666666666663</v>
       </c>
@@ -1416,9 +1415,9 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="8"/>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
+      <c r="A49" s="12"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
       <c r="D49" s="5">
         <v>0.9375</v>
       </c>
@@ -1433,9 +1432,9 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="8"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
+      <c r="A50" s="12"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
       <c r="D50" s="2">
         <v>0.95833333333333337</v>
       </c>
@@ -1450,9 +1449,9 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="8"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
+      <c r="A51" s="12"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
       <c r="D51" s="5">
         <v>0</v>
       </c>
@@ -1490,13 +1489,13 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="8" t="s">
+      <c r="A54" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B54" s="9">
+      <c r="B54" s="10">
         <v>45747</v>
       </c>
-      <c r="C54" s="9">
+      <c r="C54" s="10">
         <v>45761</v>
       </c>
       <c r="D54" s="5">
@@ -1513,9 +1512,9 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="8"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
+      <c r="A55" s="12"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
       <c r="D55" s="2">
         <v>0.4375</v>
       </c>
@@ -1530,9 +1529,9 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="8"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
+      <c r="A56" s="12"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
       <c r="D56" s="5">
         <v>0.45833333333333331</v>
       </c>
@@ -1547,9 +1546,9 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="8"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
+      <c r="A57" s="12"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
       <c r="D57" s="2">
         <v>0.91666666666666663</v>
       </c>
@@ -1564,9 +1563,9 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="8"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
+      <c r="A58" s="12"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
       <c r="D58" s="5">
         <v>0.9375</v>
       </c>
@@ -1581,9 +1580,9 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="8"/>
-      <c r="B59" s="10"/>
-      <c r="C59" s="10"/>
+      <c r="A59" s="12"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11"/>
       <c r="D59" s="2">
         <v>0.95833333333333337</v>
       </c>
@@ -1598,9 +1597,9 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="8"/>
-      <c r="B60" s="10"/>
-      <c r="C60" s="10"/>
+      <c r="A60" s="12"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="11"/>
       <c r="D60" s="5">
         <v>0</v>
       </c>
@@ -1638,13 +1637,13 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="8" t="s">
+      <c r="A63" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B63" s="9">
+      <c r="B63" s="10">
         <v>45761</v>
       </c>
-      <c r="C63" s="9">
+      <c r="C63" s="10">
         <v>45775</v>
       </c>
       <c r="D63" s="5">
@@ -1661,9 +1660,9 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="8"/>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
+      <c r="A64" s="12"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
       <c r="D64" s="2">
         <v>0.4375</v>
       </c>
@@ -1678,9 +1677,9 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="8"/>
-      <c r="B65" s="10"/>
-      <c r="C65" s="10"/>
+      <c r="A65" s="12"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
       <c r="D65" s="5">
         <v>0.45833333333333331</v>
       </c>
@@ -1695,9 +1694,9 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="8"/>
-      <c r="B66" s="10"/>
-      <c r="C66" s="10"/>
+      <c r="A66" s="12"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
       <c r="D66" s="2">
         <v>0.91666666666666663</v>
       </c>
@@ -1712,9 +1711,9 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" s="8"/>
-      <c r="B67" s="10"/>
-      <c r="C67" s="10"/>
+      <c r="A67" s="12"/>
+      <c r="B67" s="11"/>
+      <c r="C67" s="11"/>
       <c r="D67" s="5">
         <v>0.9375</v>
       </c>
@@ -1729,9 +1728,9 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="8"/>
-      <c r="B68" s="10"/>
-      <c r="C68" s="10"/>
+      <c r="A68" s="12"/>
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
       <c r="D68" s="2">
         <v>0.95833333333333337</v>
       </c>
@@ -1746,9 +1745,9 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" s="8"/>
-      <c r="B69" s="10"/>
-      <c r="C69" s="10"/>
+      <c r="A69" s="12"/>
+      <c r="B69" s="11"/>
+      <c r="C69" s="11"/>
       <c r="D69" s="5">
         <v>0</v>
       </c>
@@ -1786,13 +1785,13 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" s="8" t="s">
+      <c r="A72" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B72" s="9">
+      <c r="B72" s="10">
         <v>45775</v>
       </c>
-      <c r="C72" s="9">
+      <c r="C72" s="10">
         <v>45789</v>
       </c>
       <c r="D72" s="5">
@@ -1809,9 +1808,9 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" s="8"/>
-      <c r="B73" s="10"/>
-      <c r="C73" s="10"/>
+      <c r="A73" s="12"/>
+      <c r="B73" s="11"/>
+      <c r="C73" s="11"/>
       <c r="D73" s="2">
         <v>0.4375</v>
       </c>
@@ -1826,9 +1825,9 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="8"/>
-      <c r="B74" s="10"/>
-      <c r="C74" s="10"/>
+      <c r="A74" s="12"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="11"/>
       <c r="D74" s="5">
         <v>0.45833333333333331</v>
       </c>
@@ -1843,9 +1842,9 @@
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75" s="8"/>
-      <c r="B75" s="10"/>
-      <c r="C75" s="10"/>
+      <c r="A75" s="12"/>
+      <c r="B75" s="11"/>
+      <c r="C75" s="11"/>
       <c r="D75" s="2">
         <v>0.91666666666666663</v>
       </c>
@@ -1860,9 +1859,9 @@
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A76" s="8"/>
-      <c r="B76" s="10"/>
-      <c r="C76" s="10"/>
+      <c r="A76" s="12"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
       <c r="D76" s="5">
         <v>0.9375</v>
       </c>
@@ -1877,9 +1876,9 @@
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A77" s="8"/>
-      <c r="B77" s="10"/>
-      <c r="C77" s="10"/>
+      <c r="A77" s="12"/>
+      <c r="B77" s="11"/>
+      <c r="C77" s="11"/>
       <c r="D77" s="2">
         <v>0.95833333333333337</v>
       </c>
@@ -1894,9 +1893,9 @@
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A78" s="8"/>
-      <c r="B78" s="10"/>
-      <c r="C78" s="10"/>
+      <c r="A78" s="12"/>
+      <c r="B78" s="11"/>
+      <c r="C78" s="11"/>
       <c r="D78" s="5">
         <v>0</v>
       </c>
@@ -1934,13 +1933,13 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81" s="8" t="s">
+      <c r="A81" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B81" s="9">
+      <c r="B81" s="10">
         <v>45789</v>
       </c>
-      <c r="C81" s="9">
+      <c r="C81" s="10">
         <v>45803</v>
       </c>
       <c r="D81" s="5">
@@ -1957,9 +1956,9 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" s="8"/>
-      <c r="B82" s="10"/>
-      <c r="C82" s="10"/>
+      <c r="A82" s="12"/>
+      <c r="B82" s="11"/>
+      <c r="C82" s="11"/>
       <c r="D82" s="2">
         <v>0.4375</v>
       </c>
@@ -1974,9 +1973,9 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A83" s="8"/>
-      <c r="B83" s="10"/>
-      <c r="C83" s="10"/>
+      <c r="A83" s="12"/>
+      <c r="B83" s="11"/>
+      <c r="C83" s="11"/>
       <c r="D83" s="5">
         <v>0.45833333333333331</v>
       </c>
@@ -1991,9 +1990,9 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84" s="8"/>
-      <c r="B84" s="10"/>
-      <c r="C84" s="10"/>
+      <c r="A84" s="12"/>
+      <c r="B84" s="11"/>
+      <c r="C84" s="11"/>
       <c r="D84" s="2">
         <v>0.91666666666666663</v>
       </c>
@@ -2008,9 +2007,9 @@
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" s="8"/>
-      <c r="B85" s="10"/>
-      <c r="C85" s="10"/>
+      <c r="A85" s="12"/>
+      <c r="B85" s="11"/>
+      <c r="C85" s="11"/>
       <c r="D85" s="5">
         <v>0.9375</v>
       </c>
@@ -2025,9 +2024,9 @@
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86" s="8"/>
-      <c r="B86" s="10"/>
-      <c r="C86" s="10"/>
+      <c r="A86" s="12"/>
+      <c r="B86" s="11"/>
+      <c r="C86" s="11"/>
       <c r="D86" s="2">
         <v>0.95833333333333337</v>
       </c>
@@ -2042,9 +2041,9 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" s="8"/>
-      <c r="B87" s="10"/>
-      <c r="C87" s="10"/>
+      <c r="A87" s="12"/>
+      <c r="B87" s="11"/>
+      <c r="C87" s="11"/>
       <c r="D87" s="5">
         <v>0</v>
       </c>
@@ -2060,6 +2059,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="A45:A51"/>
+    <mergeCell ref="A36:A42"/>
+    <mergeCell ref="A9:A15"/>
+    <mergeCell ref="B9:B15"/>
+    <mergeCell ref="C9:C15"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="C18:C24"/>
+    <mergeCell ref="B27:B33"/>
+    <mergeCell ref="C27:C33"/>
+    <mergeCell ref="B36:B42"/>
+    <mergeCell ref="C36:C42"/>
     <mergeCell ref="B72:B78"/>
     <mergeCell ref="C72:C78"/>
     <mergeCell ref="B81:B87"/>
@@ -2076,20 +2089,6 @@
     <mergeCell ref="C54:C60"/>
     <mergeCell ref="B63:B69"/>
     <mergeCell ref="C63:C69"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="A45:A51"/>
-    <mergeCell ref="A36:A42"/>
-    <mergeCell ref="A9:A15"/>
-    <mergeCell ref="B9:B15"/>
-    <mergeCell ref="C9:C15"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="C18:C24"/>
-    <mergeCell ref="B27:B33"/>
-    <mergeCell ref="C27:C33"/>
-    <mergeCell ref="B36:B42"/>
-    <mergeCell ref="C36:C42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2148,22 +2147,22 @@
       <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="8">
         <v>7.7</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="8">
         <v>11.1</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="8">
         <v>8.9</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="8">
         <v>12</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="8">
         <v>70</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2174,22 +2173,22 @@
       <c r="B3" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="8">
         <v>9.5</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="8">
         <v>12.9</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="8">
         <v>11</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="8">
         <v>14</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="8">
         <v>653</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2200,22 +2199,22 @@
       <c r="B4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="8">
         <v>12.5</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="8">
         <v>14.5</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="8">
         <v>13.3</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="8">
         <v>13.2</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="8">
         <v>702</v>
       </c>
-      <c r="H4" s="12"/>
+      <c r="H4" s="9"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -2224,22 +2223,22 @@
       <c r="B5" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="8">
         <v>14.5</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="8">
         <v>16.600000000000001</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="8">
         <v>15.3</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="8">
         <v>13.4</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="8">
         <v>205</v>
       </c>
-      <c r="H5" s="12"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -2248,22 +2247,22 @@
       <c r="B6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="8">
         <v>14.5</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="8">
         <v>16.600000000000001</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="8">
         <v>15.3</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="8">
         <v>13.1</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="8">
         <v>141</v>
       </c>
-      <c r="H6" s="12"/>
+      <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -2272,22 +2271,22 @@
       <c r="B7" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="8">
         <v>17.3</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="8">
         <v>20.6</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="8">
         <v>18.2</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="8">
         <v>12.9</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="8">
         <v>196</v>
       </c>
-      <c r="H7" s="12"/>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -2296,22 +2295,22 @@
       <c r="B8" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="8">
         <v>18.100000000000001</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="8">
         <v>21.6</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="8">
         <v>19.3</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="8">
         <v>13.7</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="8">
         <v>250</v>
       </c>
-      <c r="H8" s="12"/>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -2320,22 +2319,22 @@
       <c r="B9" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="8">
         <v>18.100000000000001</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="8">
         <v>21.2</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="8">
         <v>19.2</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="8">
         <v>13.3</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="8">
         <v>265</v>
       </c>
-      <c r="H9" s="12"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -2344,22 +2343,22 @@
       <c r="B10" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="8">
         <v>18.7</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="8">
         <v>21.3</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="8">
         <v>19.7</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="8">
         <v>12.6</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="8">
         <v>280</v>
       </c>
-      <c r="H10" s="12"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -2368,22 +2367,22 @@
       <c r="B11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="8">
         <v>17.2</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="8">
         <v>20.3</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="8">
         <v>18.2</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="8">
         <v>12.1</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="8">
         <v>174</v>
       </c>
-      <c r="H11" s="12"/>
+      <c r="H11" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>